<commit_message>
Added empirical runtime data for enhanced dnc
</commit_message>
<xml_diff>
--- a/Empirical Runtime Data.xlsx
+++ b/Empirical Runtime Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">Brute Force</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">Enhanced DNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trial 9 clear outlier</t>
   </si>
 </sst>
 </file>
@@ -303,7 +300,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,7 +345,7 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -417,57 +414,195 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>3.9E-005</v>
+        <v>3.67165E-005</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>3.8E-005</v>
+        <v>2.93255E-005</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>4.3E-005</v>
+        <v>2.40803E-005</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>3.8E-005</v>
+        <v>2.36034E-005</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>4.5E-005</v>
+        <v>1.97887E-005</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>5.8E-005</v>
+        <v>1.81198E-005</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>3.9E-005</v>
+        <v>1.57356E-005</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>5.5E-005</v>
+        <v>1.90735E-005</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.000137</v>
+        <v>1.71661E-005</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>5.7E-005</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>20</v>
-      </c>
+        <v>1.71661E-005</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">AVERAGE(B14:K14)</f>
+        <v>2.207755E-005</v>
+      </c>
+      <c r="M14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <v>0.0002672672</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.0002603531</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.0002534389</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.0002527237</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.0002527237</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0.0002577305</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0.0002548695</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0.0002617836</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0.0002522469</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.0002596378</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">AVERAGE(B15:K15)</f>
+        <v>0.00025727749</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B16" s="0" t="n">
+        <v>0.0189437866</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.0185317993</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.0185585022</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.0186450481</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.0185697079</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0.0185995102</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0.0186738968</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0.0186161995</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0.0185492039</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0.0200004578</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">AVERAGE(B16:K16)</f>
+        <v>0.01876881123</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B17" s="0" t="n">
+        <v>1.90036726</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1.9290881157</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1.9752721786</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2.0134222507</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1.9555208683</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1.9984002113</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1.9526746273</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1.9439589977</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>1.9800419807</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>1.9200298786</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">AVERAGE(B17:K17)</f>
+        <v>1.95687763689</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>520.0134701729</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>463.6133487225</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>381.1040716171</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>567.3169505596</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>486.6429803371</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>509.2805206776</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>543.4538860321</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>496.919598341</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>525.3025047779</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>515.0943915844</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <f aca="false">AVERAGE(B18:K18)</f>
+        <v>500.87417228222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed errors on divide_conquer.py
</commit_message>
<xml_diff>
--- a/Empirical Runtime Data.xlsx
+++ b/Empirical Runtime Data.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Brute Force</t>
   </si>
   <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trial 1 (s)</t>
   </si>
   <si>
@@ -58,22 +61,7 @@
     <t xml:space="preserve">Average (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n = 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n = 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n = 1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n = 10000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n = 100000</t>
+    <t xml:space="preserve">Points for Graph</t>
   </si>
   <si>
     <t xml:space="preserve">Naive DNC</t>
@@ -297,15 +285,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,265 +335,292 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
+      <c r="B2" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
+      <c r="B3" s="1" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
+      <c r="B4" s="1" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
+      <c r="B5" s="1" t="n">
+        <v>10000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
+      <c r="B6" s="1" t="n">
+        <v>100000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
+      <c r="B8" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
+      <c r="B9" s="1" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
+      <c r="B10" s="1" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
+      <c r="B11" s="1" t="n">
+        <v>10000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
+      <c r="B12" s="1" t="n">
+        <v>100000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="n">
         <v>3.67165E-005</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>2.93255E-005</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>2.40803E-005</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>2.36034E-005</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>1.97887E-005</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>1.81198E-005</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="I14" s="1" t="n">
         <v>1.57356E-005</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="J14" s="1" t="n">
         <v>1.90735E-005</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>1.71661E-005</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="L14" s="1" t="n">
         <v>1.71661E-005</v>
       </c>
-      <c r="L14" s="0" t="n">
-        <f aca="false">AVERAGE(B14:K14)</f>
+      <c r="M14" s="1" t="n">
+        <f aca="false">AVERAGE(C14:L14)</f>
         <v>2.207755E-005</v>
       </c>
-      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="str">
+        <f aca="false">"(" &amp; B14 &amp; ", " &amp; M14 &amp; ")"</f>
+        <v>(10, 0.00002207755)</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1" t="n">
         <v>0.0002672672</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>0.0002603531</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>0.0002534389</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>0.0002527237</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>0.0002527237</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>0.0002577305</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="I15" s="1" t="n">
         <v>0.0002548695</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="J15" s="1" t="n">
         <v>0.0002617836</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>0.0002522469</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="L15" s="1" t="n">
         <v>0.0002596378</v>
       </c>
-      <c r="L15" s="0" t="n">
-        <f aca="false">AVERAGE(B15:K15)</f>
+      <c r="M15" s="1" t="n">
+        <f aca="false">AVERAGE(C15:L15)</f>
         <v>0.00025727749</v>
       </c>
+      <c r="N15" s="1" t="str">
+        <f aca="false">"(" &amp; B15 &amp; ", " &amp; M15 &amp; ")"</f>
+        <v>(100, 0.00025727749)</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>0.0189437866</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>0.0185317993</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>0.0185585022</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>0.0186450481</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>0.0185697079</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>0.0185995102</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="I16" s="1" t="n">
         <v>0.0186738968</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="J16" s="1" t="n">
         <v>0.0186161995</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="K16" s="1" t="n">
         <v>0.0185492039</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="L16" s="1" t="n">
         <v>0.0200004578</v>
       </c>
-      <c r="L16" s="0" t="n">
-        <f aca="false">AVERAGE(B16:K16)</f>
+      <c r="M16" s="1" t="n">
+        <f aca="false">AVERAGE(C16:L16)</f>
         <v>0.01876881123</v>
       </c>
+      <c r="N16" s="1" t="str">
+        <f aca="false">"(" &amp; B16 &amp; ", " &amp; M16 &amp; ")"</f>
+        <v>(1000, 0.01876881123)</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>1.90036726</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>1.9290881157</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>1.9752721786</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>2.0134222507</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>1.9555208683</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>1.9984002113</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="I17" s="1" t="n">
         <v>1.9526746273</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="J17" s="1" t="n">
         <v>1.9439589977</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="K17" s="1" t="n">
         <v>1.9800419807</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="L17" s="1" t="n">
         <v>1.9200298786</v>
       </c>
-      <c r="L17" s="0" t="n">
-        <f aca="false">AVERAGE(B17:K17)</f>
+      <c r="M17" s="1" t="n">
+        <f aca="false">AVERAGE(C17:L17)</f>
         <v>1.95687763689</v>
       </c>
+      <c r="N17" s="1" t="str">
+        <f aca="false">"(" &amp; B17 &amp; ", " &amp; M17 &amp; ")"</f>
+        <v>(10000, 1.95687763689)</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C18" s="1" t="n">
         <v>520.0134701729</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>463.6133487225</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>381.1040716171</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>567.3169505596</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>486.6429803371</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>509.2805206776</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="I18" s="1" t="n">
         <v>543.4538860321</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="J18" s="1" t="n">
         <v>496.919598341</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="K18" s="1" t="n">
         <v>525.3025047779</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="L18" s="1" t="n">
         <v>515.0943915844</v>
       </c>
-      <c r="L18" s="0" t="n">
-        <f aca="false">AVERAGE(B18:K18)</f>
+      <c r="M18" s="1" t="n">
+        <f aca="false">AVERAGE(C18:L18)</f>
         <v>500.87417228222</v>
       </c>
+      <c r="N18" s="1" t="str">
+        <f aca="false">"(" &amp; B18 &amp; ", " &amp; M18 &amp; ")"</f>
+        <v>(100000, 500.87417228222)</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Code optimization on DNC algos
</commit_message>
<xml_diff>
--- a/Empirical Runtime Data.xlsx
+++ b/Empirical Runtime Data.xlsx
@@ -173,43 +173,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,7 +404,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -674,65 +674,215 @@
       <c r="B8" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="M8" s="8" t="e">
+      <c r="C8" s="3" t="n">
+        <v>7.58171E-005</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>8.46386E-005</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>6.29425E-005</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>6.58035E-005</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>4.79221E-005</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>6.74725E-005</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>5.88894E-005</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>4.79221E-005</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>4.81606E-005</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>4.41074E-005</v>
+      </c>
+      <c r="M8" s="8" t="n">
         <f aca="false">AVERAGE(C8:L8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N8" s="9" t="e">
+        <v>6.036758E-005</v>
+      </c>
+      <c r="N8" s="9" t="str">
         <f aca="false">"(" &amp; B8 &amp; ", " &amp; M8 &amp; ")"</f>
-        <v>#DIV/0!</v>
+        <v>(10, 0.00006036758)</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="M9" s="8" t="e">
+      <c r="C9" s="3" t="n">
+        <v>0.0003962517</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0.0003905296</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.0003988743</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0.0003976822</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0.0004045963</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0.0004787445</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0.0003905296</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0.0003900528</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0.0003917217</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>0.0003886223</v>
+      </c>
+      <c r="M9" s="8" t="n">
         <f aca="false">AVERAGE(C9:L9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="9" t="e">
+        <v>0.0004027605</v>
+      </c>
+      <c r="N9" s="9" t="str">
         <f aca="false">"(" &amp; B9 &amp; ", " &amp; M9 &amp; ")"</f>
-        <v>#DIV/0!</v>
+        <v>(100, 0.0004027605)</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="7" t="n">
         <v>1000</v>
       </c>
-      <c r="M10" s="8" t="e">
+      <c r="C10" s="3" t="n">
+        <v>0.0039718151</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0.0040888786</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0.0041782856</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0.0038986206</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>0.0038070679</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0.0047163963</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0.003872633</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0.0037899017</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0.0037956238</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0.004267931</v>
+      </c>
+      <c r="M10" s="8" t="n">
         <f aca="false">AVERAGE(C10:L10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" s="9" t="e">
+        <v>0.00403871536</v>
+      </c>
+      <c r="N10" s="9" t="str">
         <f aca="false">"(" &amp; B10 &amp; ", " &amp; M10 &amp; ")"</f>
-        <v>#DIV/0!</v>
+        <v>(1000, 0.00403871536)</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="7" t="n">
         <v>10000</v>
       </c>
-      <c r="M11" s="8" t="e">
+      <c r="C11" s="3" t="n">
+        <v>0.0472183228</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0.0450963974</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0.0452141762</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0.044169426</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0.0440707207</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0.0443511009</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>0.0443711281</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>0.0441226959</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>0.044062376</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>0.0492372513</v>
+      </c>
+      <c r="M11" s="8" t="n">
         <f aca="false">AVERAGE(C11:L11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="9" t="e">
+        <v>0.04519135953</v>
+      </c>
+      <c r="N11" s="9" t="str">
         <f aca="false">"(" &amp; B11 &amp; ", " &amp; M11 &amp; ")"</f>
-        <v>#DIV/0!</v>
+        <v>(10000, 0.04519135953)</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="7" t="n">
         <v>100000</v>
       </c>
-      <c r="M12" s="8" t="e">
+      <c r="C12" s="3" t="n">
+        <v>0.5273954868</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0.5369346142</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>0.5256202221</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>0.5384941101</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>0.5620825291</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>0.5287666321</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>0.5310969353</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>0.5618369579</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>0.5255272388</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>0.533427</v>
+      </c>
+      <c r="M12" s="8" t="n">
         <f aca="false">AVERAGE(C12:L12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" s="9" t="e">
+        <v>0.53711817264</v>
+      </c>
+      <c r="N12" s="9" t="str">
         <f aca="false">"(" &amp; B12 &amp; ", " &amp; M12 &amp; ")"</f>
-        <v>#DIV/0!</v>
+        <v>(100000, 0.53711817264)</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -747,42 +897,42 @@
         <v>10</v>
       </c>
       <c r="C14" s="8" t="n">
+        <v>6.93798E-005</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>5.50747E-005</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>4.36306E-005</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>4.50611E-005</v>
+      </c>
+      <c r="G14" s="8" t="n">
         <v>3.67165E-005</v>
       </c>
-      <c r="D14" s="8" t="n">
-        <v>2.93255E-005</v>
-      </c>
-      <c r="E14" s="8" t="n">
-        <v>2.40803E-005</v>
-      </c>
-      <c r="F14" s="8" t="n">
-        <v>2.36034E-005</v>
-      </c>
-      <c r="G14" s="8" t="n">
-        <v>1.97887E-005</v>
-      </c>
       <c r="H14" s="8" t="n">
-        <v>1.81198E-005</v>
+        <v>4.43459E-005</v>
       </c>
       <c r="I14" s="8" t="n">
-        <v>1.57356E-005</v>
+        <v>3.50475E-005</v>
       </c>
       <c r="J14" s="8" t="n">
-        <v>1.90735E-005</v>
+        <v>3.88622E-005</v>
       </c>
       <c r="K14" s="8" t="n">
-        <v>1.71661E-005</v>
+        <v>3.40939E-005</v>
       </c>
       <c r="L14" s="8" t="n">
-        <v>1.71661E-005</v>
+        <v>3.33786E-005</v>
       </c>
       <c r="M14" s="8" t="n">
         <f aca="false">AVERAGE(C14:L14)</f>
-        <v>2.207755E-005</v>
+        <v>4.355908E-005</v>
       </c>
       <c r="N14" s="9" t="str">
         <f aca="false">"(" &amp; B14 &amp; ", " &amp; M14 &amp; ")"</f>
-        <v>(10, 0.00002207755)</v>
+        <v>(10, 0.00004355908)</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -790,42 +940,42 @@
         <v>100</v>
       </c>
       <c r="C15" s="8" t="n">
-        <v>0.0002672672</v>
+        <v>0.0003170967</v>
       </c>
       <c r="D15" s="8" t="n">
-        <v>0.0002603531</v>
+        <v>0.0003116131</v>
       </c>
       <c r="E15" s="8" t="n">
-        <v>0.0002534389</v>
+        <v>0.0003144741</v>
       </c>
       <c r="F15" s="8" t="n">
-        <v>0.0002527237</v>
+        <v>0.0003049374</v>
       </c>
       <c r="G15" s="8" t="n">
-        <v>0.0002527237</v>
+        <v>0.0003147125</v>
       </c>
       <c r="H15" s="8" t="n">
-        <v>0.0002577305</v>
+        <v>0.000305891</v>
       </c>
       <c r="I15" s="8" t="n">
-        <v>0.0002548695</v>
+        <v>0.0003020763</v>
       </c>
       <c r="J15" s="8" t="n">
-        <v>0.0002617836</v>
+        <v>0.0003089905</v>
       </c>
       <c r="K15" s="8" t="n">
-        <v>0.0002522469</v>
+        <v>0.0002975464</v>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0002596378</v>
+        <v>0.0003061295</v>
       </c>
       <c r="M15" s="8" t="n">
         <f aca="false">AVERAGE(C15:L15)</f>
-        <v>0.00025727749</v>
+        <v>0.00030834675</v>
       </c>
       <c r="N15" s="9" t="str">
         <f aca="false">"(" &amp; B15 &amp; ", " &amp; M15 &amp; ")"</f>
-        <v>(100, 0.00025727749)</v>
+        <v>(100, 0.00030834675)</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -833,42 +983,42 @@
         <v>1000</v>
       </c>
       <c r="C16" s="8" t="n">
-        <v>0.0189437866</v>
+        <v>0.0032274723</v>
       </c>
       <c r="D16" s="8" t="n">
-        <v>0.0185317993</v>
+        <v>0.0031468868</v>
       </c>
       <c r="E16" s="8" t="n">
-        <v>0.0185585022</v>
+        <v>0.0032169819</v>
       </c>
       <c r="F16" s="8" t="n">
-        <v>0.0186450481</v>
+        <v>0.0031776428</v>
       </c>
       <c r="G16" s="8" t="n">
-        <v>0.0185697079</v>
+        <v>0.0031192303</v>
       </c>
       <c r="H16" s="8" t="n">
-        <v>0.0185995102</v>
+        <v>0.0031518936</v>
       </c>
       <c r="I16" s="8" t="n">
-        <v>0.0186738968</v>
+        <v>0.0031163692</v>
       </c>
       <c r="J16" s="8" t="n">
-        <v>0.0186161995</v>
+        <v>0.0031385422</v>
       </c>
       <c r="K16" s="8" t="n">
-        <v>0.0185492039</v>
+        <v>0.0031421185</v>
       </c>
       <c r="L16" s="8" t="n">
-        <v>0.0200004578</v>
+        <v>0.0031671524</v>
       </c>
       <c r="M16" s="8" t="n">
         <f aca="false">AVERAGE(C16:L16)</f>
-        <v>0.01876881123</v>
+        <v>0.003160429</v>
       </c>
       <c r="N16" s="9" t="str">
         <f aca="false">"(" &amp; B16 &amp; ", " &amp; M16 &amp; ")"</f>
-        <v>(1000, 0.01876881123)</v>
+        <v>(1000, 0.003160429)</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -876,42 +1026,42 @@
         <v>10000</v>
       </c>
       <c r="C17" s="8" t="n">
-        <v>1.90036726</v>
+        <v>0.0406410694</v>
       </c>
       <c r="D17" s="8" t="n">
-        <v>1.9290881157</v>
+        <v>0.0405409336</v>
       </c>
       <c r="E17" s="8" t="n">
-        <v>1.9752721786</v>
+        <v>0.0405299664</v>
       </c>
       <c r="F17" s="8" t="n">
-        <v>2.0134222507</v>
+        <v>0.0406548977</v>
       </c>
       <c r="G17" s="8" t="n">
-        <v>1.9555208683</v>
+        <v>0.0405220985</v>
       </c>
       <c r="H17" s="8" t="n">
-        <v>1.9984002113</v>
+        <v>0.0406138897</v>
       </c>
       <c r="I17" s="8" t="n">
-        <v>1.9526746273</v>
+        <v>0.0405135155</v>
       </c>
       <c r="J17" s="8" t="n">
-        <v>1.9439589977</v>
+        <v>0.0411868095</v>
       </c>
       <c r="K17" s="8" t="n">
-        <v>1.9800419807</v>
+        <v>0.0406839848</v>
       </c>
       <c r="L17" s="8" t="n">
-        <v>1.9200298786</v>
+        <v>0.0405249596</v>
       </c>
       <c r="M17" s="8" t="n">
         <f aca="false">AVERAGE(C17:L17)</f>
-        <v>1.95687763689</v>
+        <v>0.04064121247</v>
       </c>
       <c r="N17" s="9" t="str">
         <f aca="false">"(" &amp; B17 &amp; ", " &amp; M17 &amp; ")"</f>
-        <v>(10000, 1.95687763689)</v>
+        <v>(10000, 0.04064121247)</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -919,45 +1069,87 @@
         <v>100000</v>
       </c>
       <c r="C18" s="8" t="n">
-        <v>520.0134701729</v>
+        <v>0.5544199944</v>
       </c>
       <c r="D18" s="8" t="n">
-        <v>463.6133487225</v>
+        <v>0.542617321</v>
       </c>
       <c r="E18" s="8" t="n">
-        <v>381.1040716171</v>
+        <v>0.5580203533</v>
       </c>
       <c r="F18" s="8" t="n">
-        <v>567.3169505596</v>
+        <v>0.5660443306</v>
       </c>
       <c r="G18" s="8" t="n">
-        <v>486.6429803371</v>
+        <v>0.5544099808</v>
       </c>
       <c r="H18" s="8" t="n">
-        <v>509.2805206776</v>
+        <v>0.5558817387</v>
       </c>
       <c r="I18" s="8" t="n">
-        <v>543.4538860321</v>
+        <v>0.5537266731</v>
       </c>
       <c r="J18" s="8" t="n">
-        <v>496.919598341</v>
+        <v>0.5552794933</v>
       </c>
       <c r="K18" s="8" t="n">
-        <v>525.3025047779</v>
+        <v>0.5548655987</v>
       </c>
       <c r="L18" s="8" t="n">
-        <v>515.0943915844</v>
+        <v>0.5699870586</v>
       </c>
       <c r="M18" s="8" t="n">
         <f aca="false">AVERAGE(C18:L18)</f>
-        <v>500.87417228222</v>
+        <v>0.55652525425</v>
       </c>
       <c r="N18" s="9" t="str">
         <f aca="false">"(" &amp; B18 &amp; ", " &amp; M18 &amp; ")"</f>
-        <v>(100000, 500.87417228222)</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>(100000, 0.55652525425)</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>9.766307354</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>9.6560795307</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>10.7907721996</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>10.0300133228</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>9.7327427864</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>10.7889122963</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>11.4387202263</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>11.5064268112</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <v>10.70480299</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>10.8377747536</v>
+      </c>
+      <c r="M19" s="8" t="n">
+        <f aca="false">AVERAGE(C19:L19)</f>
+        <v>10.52525522709</v>
+      </c>
+      <c r="N19" s="9" t="str">
+        <f aca="false">"(" &amp; B19 &amp; ", " &amp; M19 &amp; ")"</f>
+        <v>(1000000, 10.52525522709)</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update test data for naive and enhanced
</commit_message>
<xml_diff>
--- a/Empirical Runtime Data.xlsx
+++ b/Empirical Runtime Data.xlsx
@@ -404,7 +404,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -675,42 +675,42 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>7.58171E-005</v>
+        <v>4.64916E-005</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>8.46386E-005</v>
+        <v>4.69685E-005</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>6.29425E-005</v>
+        <v>4.29153E-005</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>6.58035E-005</v>
+        <v>2.47955E-005</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>4.79221E-005</v>
+        <v>2.40803E-005</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>6.74725E-005</v>
+        <v>2.55108E-005</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>5.88894E-005</v>
+        <v>2.74181E-005</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>4.79221E-005</v>
+        <v>2.57492E-005</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>4.81606E-005</v>
+        <v>2.69413E-005</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>4.41074E-005</v>
+        <v>2.40803E-005</v>
       </c>
       <c r="M8" s="8" t="n">
         <f aca="false">AVERAGE(C8:L8)</f>
-        <v>6.036758E-005</v>
+        <v>3.149509E-005</v>
       </c>
       <c r="N8" s="9" t="str">
         <f aca="false">"(" &amp; B8 &amp; ", " &amp; M8 &amp; ")"</f>
-        <v>(10, 0.00006036758)</v>
+        <v>(10, 0.00003149509)</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -718,42 +718,42 @@
         <v>100</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>0.0003962517</v>
+        <v>0.000191927</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.0003905296</v>
+        <v>0.0001952648</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.0003988743</v>
+        <v>0.0001897812</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>0.0003976822</v>
+        <v>0.0001943111</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>0.0004045963</v>
+        <v>0.0002081394</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>0.0004787445</v>
+        <v>0.0001881123</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>0.0003905296</v>
+        <v>0.0002028942</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>0.0003900528</v>
+        <v>0.0001897812</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>0.0003917217</v>
+        <v>0.0001835823</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>0.0003886223</v>
+        <v>0.0002529621</v>
       </c>
       <c r="M9" s="8" t="n">
         <f aca="false">AVERAGE(C9:L9)</f>
-        <v>0.0004027605</v>
+        <v>0.00019967556</v>
       </c>
       <c r="N9" s="9" t="str">
         <f aca="false">"(" &amp; B9 &amp; ", " &amp; M9 &amp; ")"</f>
-        <v>(100, 0.0004027605)</v>
+        <v>(100, 0.00019967556)</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -761,42 +761,42 @@
         <v>1000</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>0.0039718151</v>
+        <v>0.0021913052</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.0040888786</v>
+        <v>0.0021038055</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0.0041782856</v>
+        <v>0.002051115</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0.0038986206</v>
+        <v>0.0020518303</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>0.0038070679</v>
+        <v>0.0020358562</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>0.0047163963</v>
+        <v>0.0020914078</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>0.003872633</v>
+        <v>0.0020909309</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>0.0037899017</v>
+        <v>0.0020787716</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>0.0037956238</v>
+        <v>0.0021634102</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0.004267931</v>
+        <v>0.0021250248</v>
       </c>
       <c r="M10" s="8" t="n">
         <f aca="false">AVERAGE(C10:L10)</f>
-        <v>0.00403871536</v>
+        <v>0.00209834575</v>
       </c>
       <c r="N10" s="9" t="str">
         <f aca="false">"(" &amp; B10 &amp; ", " &amp; M10 &amp; ")"</f>
-        <v>(1000, 0.00403871536)</v>
+        <v>(1000, 0.00209834575)</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -804,42 +804,42 @@
         <v>10000</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>0.0472183228</v>
+        <v>0.0251362324</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0.0450963974</v>
+        <v>0.0265309811</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0.0452141762</v>
+        <v>0.0254600048</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0.044169426</v>
+        <v>0.0249166489</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>0.0440707207</v>
+        <v>0.0249860287</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>0.0443511009</v>
+        <v>0.0255236626</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>0.0443711281</v>
+        <v>0.0251948833</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>0.0441226959</v>
+        <v>0.025187254</v>
       </c>
       <c r="K11" s="3" t="n">
-        <v>0.044062376</v>
+        <v>0.0250411034</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>0.0492372513</v>
+        <v>0.0250582695</v>
       </c>
       <c r="M11" s="8" t="n">
         <f aca="false">AVERAGE(C11:L11)</f>
-        <v>0.04519135953</v>
+        <v>0.02530350687</v>
       </c>
       <c r="N11" s="9" t="str">
         <f aca="false">"(" &amp; B11 &amp; ", " &amp; M11 &amp; ")"</f>
-        <v>(10000, 0.04519135953)</v>
+        <v>(10000, 0.02530350687)</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -847,42 +847,42 @@
         <v>100000</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>0.5273954868</v>
+        <v>0.3355109692</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.5369346142</v>
+        <v>0.325835228</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0.5256202221</v>
+        <v>0.3291053772</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.5384941101</v>
+        <v>0.3261523247</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>0.5620825291</v>
+        <v>0.3278408051</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>0.5287666321</v>
+        <v>0.3202004433</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>0.5310969353</v>
+        <v>0.3270783424</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>0.5618369579</v>
+        <v>0.3341903687</v>
       </c>
       <c r="K12" s="3" t="n">
-        <v>0.5255272388</v>
+        <v>0.3430426121</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>0.533427</v>
+        <v>0.3250625134</v>
       </c>
       <c r="M12" s="8" t="n">
         <f aca="false">AVERAGE(C12:L12)</f>
-        <v>0.53711817264</v>
+        <v>0.32940189841</v>
       </c>
       <c r="N12" s="9" t="str">
         <f aca="false">"(" &amp; B12 &amp; ", " &amp; M12 &amp; ")"</f>
-        <v>(100000, 0.53711817264)</v>
+        <v>(100000, 0.32940189841)</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -897,42 +897,42 @@
         <v>10</v>
       </c>
       <c r="C14" s="8" t="n">
-        <v>6.93798E-005</v>
+        <v>4.62532E-005</v>
       </c>
       <c r="D14" s="8" t="n">
-        <v>5.50747E-005</v>
+        <v>3.60012E-005</v>
       </c>
       <c r="E14" s="8" t="n">
-        <v>4.36306E-005</v>
+        <v>2.88486E-005</v>
       </c>
       <c r="F14" s="8" t="n">
-        <v>4.50611E-005</v>
+        <v>2.36034E-005</v>
       </c>
       <c r="G14" s="8" t="n">
-        <v>3.67165E-005</v>
+        <v>2.24113E-005</v>
       </c>
       <c r="H14" s="8" t="n">
-        <v>4.43459E-005</v>
+        <v>1.95503E-005</v>
       </c>
       <c r="I14" s="8" t="n">
-        <v>3.50475E-005</v>
+        <v>2.0504E-005</v>
       </c>
       <c r="J14" s="8" t="n">
-        <v>3.88622E-005</v>
+        <v>2.59876E-005</v>
       </c>
       <c r="K14" s="8" t="n">
-        <v>3.40939E-005</v>
+        <v>2.19345E-005</v>
       </c>
       <c r="L14" s="8" t="n">
-        <v>3.33786E-005</v>
+        <v>2.07424E-005</v>
       </c>
       <c r="M14" s="8" t="n">
         <f aca="false">AVERAGE(C14:L14)</f>
-        <v>4.355908E-005</v>
+        <v>2.658365E-005</v>
       </c>
       <c r="N14" s="9" t="str">
         <f aca="false">"(" &amp; B14 &amp; ", " &amp; M14 &amp; ")"</f>
-        <v>(10, 0.00004355908)</v>
+        <v>(10, 0.00002658365)</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -940,42 +940,42 @@
         <v>100</v>
       </c>
       <c r="C15" s="8" t="n">
-        <v>0.0003170967</v>
+        <v>0.000194788</v>
       </c>
       <c r="D15" s="8" t="n">
-        <v>0.0003116131</v>
+        <v>0.0001869202</v>
       </c>
       <c r="E15" s="8" t="n">
-        <v>0.0003144741</v>
+        <v>0.0001864433</v>
       </c>
       <c r="F15" s="8" t="n">
-        <v>0.0003049374</v>
+        <v>0.0001823902</v>
       </c>
       <c r="G15" s="8" t="n">
-        <v>0.0003147125</v>
+        <v>0.0001888275</v>
       </c>
       <c r="H15" s="8" t="n">
-        <v>0.000305891</v>
+        <v>0.000180006</v>
       </c>
       <c r="I15" s="8" t="n">
-        <v>0.0003020763</v>
+        <v>0.0001823902</v>
       </c>
       <c r="J15" s="8" t="n">
-        <v>0.0003089905</v>
+        <v>0.000181675</v>
       </c>
       <c r="K15" s="8" t="n">
-        <v>0.0002975464</v>
+        <v>0.000171423</v>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0003061295</v>
+        <v>0.0001797676</v>
       </c>
       <c r="M15" s="8" t="n">
         <f aca="false">AVERAGE(C15:L15)</f>
-        <v>0.00030834675</v>
+        <v>0.0001834631</v>
       </c>
       <c r="N15" s="9" t="str">
         <f aca="false">"(" &amp; B15 &amp; ", " &amp; M15 &amp; ")"</f>
-        <v>(100, 0.00030834675)</v>
+        <v>(100, 0.0001834631)</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -983,42 +983,42 @@
         <v>1000</v>
       </c>
       <c r="C16" s="8" t="n">
-        <v>0.0032274723</v>
+        <v>0.0021557808</v>
       </c>
       <c r="D16" s="8" t="n">
-        <v>0.0031468868</v>
+        <v>0.0020956993</v>
       </c>
       <c r="E16" s="8" t="n">
-        <v>0.0032169819</v>
+        <v>0.0021114349</v>
       </c>
       <c r="F16" s="8" t="n">
-        <v>0.0031776428</v>
+        <v>0.0021185875</v>
       </c>
       <c r="G16" s="8" t="n">
-        <v>0.0031192303</v>
+        <v>0.0021226406</v>
       </c>
       <c r="H16" s="8" t="n">
-        <v>0.0031518936</v>
+        <v>0.0021467209</v>
       </c>
       <c r="I16" s="8" t="n">
-        <v>0.0031163692</v>
+        <v>0.0021729469</v>
       </c>
       <c r="J16" s="8" t="n">
-        <v>0.0031385422</v>
+        <v>0.0021443367</v>
       </c>
       <c r="K16" s="8" t="n">
-        <v>0.0031421185</v>
+        <v>0.0021195412</v>
       </c>
       <c r="L16" s="8" t="n">
-        <v>0.0031671524</v>
+        <v>0.0021443367</v>
       </c>
       <c r="M16" s="8" t="n">
         <f aca="false">AVERAGE(C16:L16)</f>
-        <v>0.003160429</v>
+        <v>0.00213320255</v>
       </c>
       <c r="N16" s="9" t="str">
         <f aca="false">"(" &amp; B16 &amp; ", " &amp; M16 &amp; ")"</f>
-        <v>(1000, 0.003160429)</v>
+        <v>(1000, 0.00213320255)</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1026,42 +1026,42 @@
         <v>10000</v>
       </c>
       <c r="C17" s="8" t="n">
-        <v>0.0406410694</v>
+        <v>0.0275919437</v>
       </c>
       <c r="D17" s="8" t="n">
-        <v>0.0405409336</v>
+        <v>0.0272498131</v>
       </c>
       <c r="E17" s="8" t="n">
-        <v>0.0405299664</v>
+        <v>0.0275504589</v>
       </c>
       <c r="F17" s="8" t="n">
-        <v>0.0406548977</v>
+        <v>0.0275506973</v>
       </c>
       <c r="G17" s="8" t="n">
-        <v>0.0405220985</v>
+        <v>0.0276648998</v>
       </c>
       <c r="H17" s="8" t="n">
-        <v>0.0406138897</v>
+        <v>0.0274918079</v>
       </c>
       <c r="I17" s="8" t="n">
-        <v>0.0405135155</v>
+        <v>0.0277087688</v>
       </c>
       <c r="J17" s="8" t="n">
-        <v>0.0411868095</v>
+        <v>0.027971983</v>
       </c>
       <c r="K17" s="8" t="n">
-        <v>0.0406839848</v>
+        <v>0.0279300213</v>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.0405249596</v>
+        <v>0.027859211</v>
       </c>
       <c r="M17" s="8" t="n">
         <f aca="false">AVERAGE(C17:L17)</f>
-        <v>0.04064121247</v>
+        <v>0.02765696048</v>
       </c>
       <c r="N17" s="9" t="str">
         <f aca="false">"(" &amp; B17 &amp; ", " &amp; M17 &amp; ")"</f>
-        <v>(10000, 0.04064121247)</v>
+        <v>(10000, 0.02765696048)</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1069,85 +1069,52 @@
         <v>100000</v>
       </c>
       <c r="C18" s="8" t="n">
-        <v>0.5544199944</v>
+        <v>0.4755814075</v>
       </c>
       <c r="D18" s="8" t="n">
-        <v>0.542617321</v>
+        <v>0.4346909523</v>
       </c>
       <c r="E18" s="8" t="n">
-        <v>0.5580203533</v>
+        <v>0.466121912</v>
       </c>
       <c r="F18" s="8" t="n">
-        <v>0.5660443306</v>
+        <v>0.4473838806</v>
       </c>
       <c r="G18" s="8" t="n">
-        <v>0.5544099808</v>
+        <v>0.4455771446</v>
       </c>
       <c r="H18" s="8" t="n">
-        <v>0.5558817387</v>
+        <v>0.4395196438</v>
       </c>
       <c r="I18" s="8" t="n">
-        <v>0.5537266731</v>
+        <v>0.4684042931</v>
       </c>
       <c r="J18" s="8" t="n">
-        <v>0.5552794933</v>
+        <v>0.4553773403</v>
       </c>
       <c r="K18" s="8" t="n">
-        <v>0.5548655987</v>
+        <v>0.4605810642</v>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.5699870586</v>
+        <v>0.4459555149</v>
       </c>
       <c r="M18" s="8" t="n">
         <f aca="false">AVERAGE(C18:L18)</f>
-        <v>0.55652525425</v>
+        <v>0.45391931533</v>
       </c>
       <c r="N18" s="9" t="str">
         <f aca="false">"(" &amp; B18 &amp; ", " &amp; M18 &amp; ")"</f>
-        <v>(100000, 0.55652525425)</v>
+        <v>(100000, 0.45391931533)</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
         <v>1000000</v>
       </c>
-      <c r="C19" s="3" t="n">
-        <v>9.766307354</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>9.6560795307</v>
-      </c>
-      <c r="E19" s="3" t="n">
-        <v>10.7907721996</v>
-      </c>
-      <c r="F19" s="3" t="n">
-        <v>10.0300133228</v>
-      </c>
-      <c r="G19" s="3" t="n">
-        <v>9.7327427864</v>
-      </c>
-      <c r="H19" s="3" t="n">
-        <v>10.7889122963</v>
-      </c>
-      <c r="I19" s="3" t="n">
-        <v>11.4387202263</v>
-      </c>
-      <c r="J19" s="3" t="n">
-        <v>11.5064268112</v>
-      </c>
-      <c r="K19" s="3" t="n">
-        <v>10.70480299</v>
-      </c>
-      <c r="L19" s="3" t="n">
-        <v>10.8377747536</v>
-      </c>
-      <c r="M19" s="8" t="n">
-        <f aca="false">AVERAGE(C19:L19)</f>
-        <v>10.52525522709</v>
-      </c>
+      <c r="M19" s="8"/>
       <c r="N19" s="9" t="str">
         <f aca="false">"(" &amp; B19 &amp; ", " &amp; M19 &amp; ")"</f>
-        <v>(1000000, 10.52525522709)</v>
+        <v>(1000000, )</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Switched back to separate x and y arrays
</commit_message>
<xml_diff>
--- a/Empirical Runtime Data.xlsx
+++ b/Empirical Runtime Data.xlsx
@@ -404,7 +404,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -897,42 +897,41 @@
         <v>10</v>
       </c>
       <c r="C14" s="8" t="n">
-        <v>4.62532E-005</v>
+        <v>4.81606E-005</v>
       </c>
       <c r="D14" s="8" t="n">
-        <v>3.60012E-005</v>
+        <v>5.57899E-005</v>
       </c>
       <c r="E14" s="8" t="n">
+        <v>2.86102E-005</v>
+      </c>
+      <c r="F14" s="8" t="n">
         <v>2.88486E-005</v>
       </c>
-      <c r="F14" s="8" t="n">
-        <v>2.36034E-005</v>
-      </c>
       <c r="G14" s="8" t="n">
-        <v>2.24113E-005</v>
+        <v>2.38419E-005</v>
       </c>
       <c r="H14" s="8" t="n">
+        <v>2.57492E-005</v>
+      </c>
+      <c r="I14" s="8" t="n">
         <v>1.95503E-005</v>
       </c>
-      <c r="I14" s="8" t="n">
-        <v>2.0504E-005</v>
-      </c>
       <c r="J14" s="8" t="n">
-        <v>2.59876E-005</v>
+        <v>2.3365E-005</v>
       </c>
       <c r="K14" s="8" t="n">
-        <v>2.19345E-005</v>
+        <v>2.02656E-005</v>
       </c>
       <c r="L14" s="8" t="n">
-        <v>2.07424E-005</v>
+        <v>1.93119E-005</v>
       </c>
       <c r="M14" s="8" t="n">
-        <f aca="false">AVERAGE(C14:L14)</f>
-        <v>2.658365E-005</v>
+        <v>4.81606E-005</v>
       </c>
       <c r="N14" s="9" t="str">
         <f aca="false">"(" &amp; B14 &amp; ", " &amp; M14 &amp; ")"</f>
-        <v>(10, 0.00002658365)</v>
+        <v>(10, 0.0000481606)</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -940,42 +939,41 @@
         <v>100</v>
       </c>
       <c r="C15" s="8" t="n">
-        <v>0.000194788</v>
+        <v>0.0002086163</v>
       </c>
       <c r="D15" s="8" t="n">
-        <v>0.0001869202</v>
+        <v>0.0003092289</v>
       </c>
       <c r="E15" s="8" t="n">
-        <v>0.0001864433</v>
+        <v>0.0001916885</v>
       </c>
       <c r="F15" s="8" t="n">
-        <v>0.0001823902</v>
+        <v>0.0001826286</v>
       </c>
       <c r="G15" s="8" t="n">
-        <v>0.0001888275</v>
+        <v>0.0001907349</v>
       </c>
       <c r="H15" s="8" t="n">
-        <v>0.000180006</v>
+        <v>0.0001881123</v>
       </c>
       <c r="I15" s="8" t="n">
-        <v>0.0001823902</v>
+        <v>0.0001854897</v>
       </c>
       <c r="J15" s="8" t="n">
-        <v>0.000181675</v>
+        <v>0.0001833439</v>
       </c>
       <c r="K15" s="8" t="n">
-        <v>0.000171423</v>
+        <v>0.0001802444</v>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0001797676</v>
+        <v>0.000187397</v>
       </c>
       <c r="M15" s="8" t="n">
-        <f aca="false">AVERAGE(C15:L15)</f>
-        <v>0.0001834631</v>
+        <v>0.0002086163</v>
       </c>
       <c r="N15" s="9" t="str">
         <f aca="false">"(" &amp; B15 &amp; ", " &amp; M15 &amp; ")"</f>
-        <v>(100, 0.0001834631)</v>
+        <v>(100, 0.0002086163)</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -983,42 +981,41 @@
         <v>1000</v>
       </c>
       <c r="C16" s="8" t="n">
-        <v>0.0021557808</v>
+        <v>0.002692461</v>
       </c>
       <c r="D16" s="8" t="n">
-        <v>0.0020956993</v>
+        <v>0.0021409988</v>
       </c>
       <c r="E16" s="8" t="n">
-        <v>0.0021114349</v>
+        <v>0.0020980835</v>
       </c>
       <c r="F16" s="8" t="n">
-        <v>0.0021185875</v>
+        <v>0.0028743744</v>
       </c>
       <c r="G16" s="8" t="n">
-        <v>0.0021226406</v>
+        <v>0.002177</v>
       </c>
       <c r="H16" s="8" t="n">
-        <v>0.0021467209</v>
+        <v>0.0021882057</v>
       </c>
       <c r="I16" s="8" t="n">
-        <v>0.0021729469</v>
+        <v>0.0023241043</v>
       </c>
       <c r="J16" s="8" t="n">
-        <v>0.0021443367</v>
+        <v>0.0022110939</v>
       </c>
       <c r="K16" s="8" t="n">
-        <v>0.0021195412</v>
+        <v>0.0021512508</v>
       </c>
       <c r="L16" s="8" t="n">
-        <v>0.0021443367</v>
+        <v>0.0021877289</v>
       </c>
       <c r="M16" s="8" t="n">
-        <f aca="false">AVERAGE(C16:L16)</f>
-        <v>0.00213320255</v>
+        <v>0.002692461</v>
       </c>
       <c r="N16" s="9" t="str">
         <f aca="false">"(" &amp; B16 &amp; ", " &amp; M16 &amp; ")"</f>
-        <v>(1000, 0.00213320255)</v>
+        <v>(1000, 0.002692461)</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1026,42 +1023,41 @@
         <v>10000</v>
       </c>
       <c r="C17" s="8" t="n">
-        <v>0.0275919437</v>
+        <v>0.0294098854</v>
       </c>
       <c r="D17" s="8" t="n">
-        <v>0.0272498131</v>
+        <v>0.0282216072</v>
       </c>
       <c r="E17" s="8" t="n">
-        <v>0.0275504589</v>
+        <v>0.030138731</v>
       </c>
       <c r="F17" s="8" t="n">
-        <v>0.0275506973</v>
+        <v>0.0300579071</v>
       </c>
       <c r="G17" s="8" t="n">
-        <v>0.0276648998</v>
+        <v>0.0295789242</v>
       </c>
       <c r="H17" s="8" t="n">
-        <v>0.0274918079</v>
+        <v>0.0299756527</v>
       </c>
       <c r="I17" s="8" t="n">
-        <v>0.0277087688</v>
+        <v>0.0318930149</v>
       </c>
       <c r="J17" s="8" t="n">
-        <v>0.027971983</v>
+        <v>0.0303976536</v>
       </c>
       <c r="K17" s="8" t="n">
-        <v>0.0279300213</v>
+        <v>0.0294623375</v>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.027859211</v>
+        <v>0.0288746357</v>
       </c>
       <c r="M17" s="8" t="n">
-        <f aca="false">AVERAGE(C17:L17)</f>
-        <v>0.02765696048</v>
+        <v>0.0294098854</v>
       </c>
       <c r="N17" s="9" t="str">
         <f aca="false">"(" &amp; B17 &amp; ", " &amp; M17 &amp; ")"</f>
-        <v>(10000, 0.02765696048)</v>
+        <v>(10000, 0.0294098854)</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1069,42 +1065,41 @@
         <v>100000</v>
       </c>
       <c r="C18" s="8" t="n">
-        <v>0.4755814075</v>
+        <v>0.5436584949</v>
       </c>
       <c r="D18" s="8" t="n">
-        <v>0.4346909523</v>
+        <v>0.5398054123</v>
       </c>
       <c r="E18" s="8" t="n">
-        <v>0.466121912</v>
+        <v>0.6011793613</v>
       </c>
       <c r="F18" s="8" t="n">
-        <v>0.4473838806</v>
+        <v>0.5864839554</v>
       </c>
       <c r="G18" s="8" t="n">
-        <v>0.4455771446</v>
+        <v>0.6017947197</v>
       </c>
       <c r="H18" s="8" t="n">
-        <v>0.4395196438</v>
+        <v>0.5902104378</v>
       </c>
       <c r="I18" s="8" t="n">
-        <v>0.4684042931</v>
+        <v>0.5673451424</v>
       </c>
       <c r="J18" s="8" t="n">
-        <v>0.4553773403</v>
+        <v>0.6004822254</v>
       </c>
       <c r="K18" s="8" t="n">
-        <v>0.4605810642</v>
+        <v>0.573120594</v>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.4459555149</v>
+        <v>0.6028115749</v>
       </c>
       <c r="M18" s="8" t="n">
-        <f aca="false">AVERAGE(C18:L18)</f>
-        <v>0.45391931533</v>
+        <v>0.5436584949</v>
       </c>
       <c r="N18" s="9" t="str">
         <f aca="false">"(" &amp; B18 &amp; ", " &amp; M18 &amp; ")"</f>
-        <v>(100000, 0.45391931533)</v>
+        <v>(100000, 0.5436584949)</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>